<commit_message>
Detailed mesh size ranges
</commit_message>
<xml_diff>
--- a/Metiers/metier_results_summary.xlsx
+++ b/Metiers/metier_results_summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t xml:space="preserve">Country</t>
   </si>
@@ -20,7 +20,7 @@
     <t xml:space="preserve">RCG</t>
   </si>
   <si>
-    <t xml:space="preserve">metier_level_6</t>
+    <t xml:space="preserve">metier_level_6_new</t>
   </si>
   <si>
     <t xml:space="preserve">n_count</t>
@@ -50,9 +50,6 @@
     <t xml:space="preserve">LLD_ANA_0_0_0</t>
   </si>
   <si>
-    <t xml:space="preserve">LLS_DEF_0_0_0</t>
-  </si>
-  <si>
     <t xml:space="preserve">MIS_MIS_0_0_0</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
   </si>
   <si>
     <t xml:space="preserve">NSEA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OTB_DWS_100-119_0_0</t>
   </si>
 </sst>
 </file>
@@ -437,13 +431,13 @@
         <v>8</v>
       </c>
       <c r="D2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E2" t="n">
-        <v>1880</v>
+        <v>1600</v>
       </c>
       <c r="F2" t="n">
-        <v>560</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -477,13 +471,13 @@
         <v>10</v>
       </c>
       <c r="D4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E4" t="n">
-        <v>800</v>
+        <v>1080</v>
       </c>
       <c r="F4" t="n">
-        <v>1400</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="5">
@@ -520,10 +514,10 @@
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>300</v>
+        <v>20</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7">
@@ -537,13 +531,13 @@
         <v>13</v>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E7" t="n">
-        <v>20</v>
+        <v>3066</v>
       </c>
       <c r="F7" t="n">
-        <v>100</v>
+        <v>2761.2</v>
       </c>
     </row>
     <row r="8">
@@ -557,13 +551,13 @@
         <v>14</v>
       </c>
       <c r="D8" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E8" t="n">
-        <v>3066</v>
+        <v>180</v>
       </c>
       <c r="F8" t="n">
-        <v>2761.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -580,7 +574,7 @@
         <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>180</v>
+        <v>900</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -591,16 +585,16 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" t="n">
         <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>600</v>
+        <v>18000</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -611,38 +605,18 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11" t="n">
-        <v>18000</v>
+        <v>2900</v>
       </c>
       <c r="F11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="n">
-        <v>4</v>
-      </c>
-      <c r="E12" t="n">
-        <v>2900</v>
-      </c>
-      <c r="F12" t="n">
         <v>5085</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update of the markdown document and examples
</commit_message>
<xml_diff>
--- a/Metiers/metier_results_summary.xlsx
+++ b/Metiers/metier_results_summary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Country</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t xml:space="preserve">OTB_DEF_105-115_1_120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OTB_DEF_&gt;0_0_0</t>
   </si>
   <si>
     <t xml:space="preserve">OTB_DEF_&gt;=120_3_120</t>
@@ -551,10 +554,10 @@
         <v>14</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E8" t="n">
-        <v>180</v>
+        <v>1300</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -574,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="E9" t="n">
-        <v>900</v>
+        <v>180</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -585,16 +588,16 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
       </c>
       <c r="D10" t="n">
         <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>18000</v>
+        <v>600</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -605,18 +608,38 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>18000</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D12" t="n">
         <v>4</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E12" t="n">
         <v>2900</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F12" t="n">
         <v>5085</v>
       </c>
     </row>

</xml_diff>